<commit_message>
added Section info for basic staage on OutCourse
</commit_message>
<xml_diff>
--- a/区間情報/区間情報まとめ.xlsx
+++ b/区間情報/区間情報まとめ.xlsx
@@ -123,14 +123,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>SixthCurve_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SixthCurve_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>距離合計[mm]</t>
     <rPh sb="0" eb="2">
       <t>キョリ</t>
@@ -233,6 +225,14 @@
 </t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>OutSixthCurve_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OutSixthCurve_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -296,11 +296,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3507,7 +3507,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3536,32 +3536,32 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
         <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" t="s">
-        <v>31</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
@@ -3569,14 +3569,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D4">
         <v>200</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <v>1010</v>
       </c>
       <c r="G4" s="1"/>
@@ -3585,29 +3585,29 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
       <c r="D5">
         <v>810</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="1"/>
       <c r="H5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>570</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <f>SUM(D6:D7)</f>
         <v>1710</v>
       </c>
@@ -3617,21 +3617,21 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>1140</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="1"/>
       <c r="H7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -3646,7 +3646,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -3667,7 +3667,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -3682,7 +3682,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A11" s="3"/>
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -3701,12 +3701,12 @@
         <f>1/H11</f>
         <v>726.76</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -3729,10 +3729,10 @@
       <c r="J12">
         <v>570</v>
       </c>
-      <c r="K12" s="3"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -3754,10 +3754,10 @@
         <f>1/H13</f>
         <v>927.14831999999979</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
+      <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -3769,28 +3769,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <f>(1/H15)*(PI()/180)*G15</f>
         <v>299.21924696190786</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>21.43</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <f>1/I15</f>
         <v>1.25E-3</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>800</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
+      <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>17</v>
       </c>
@@ -3810,7 +3810,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
+      <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -3831,9 +3831,9 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
+      <c r="A18" s="4"/>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -3852,9 +3852,9 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
@@ -3873,7 +3873,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
+      <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -3885,7 +3885,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A21" s="3"/>
+      <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>20</v>
       </c>
@@ -3906,7 +3906,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A22" s="3"/>
+      <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -3927,9 +3927,9 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A23" s="3"/>
+      <c r="A23" s="4"/>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D23">
         <v>1010</v>
@@ -3949,9 +3949,9 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A24" s="3"/>
+      <c r="A24" s="4"/>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24">
         <f>(1/H24)*(PI()/180)*G24</f>
@@ -3969,21 +3969,21 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="3"/>
+      <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I25">
         <v>650</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A26" s="3"/>
+      <c r="A26" s="4"/>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D26">
         <f>(1/H26)*(PI()/180)*G26</f>
@@ -4001,9 +4001,9 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A27" s="3"/>
+      <c r="A27" s="4"/>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D27">
         <f>(1/H27)*(PI()/180)*G27</f>
@@ -4038,7 +4038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>

</xml_diff>